<commit_message>
Integración con perfiles definidos
Signed-off-by: qa-katalon <qa-katalon@DEV-QA-KatalonStudio.BMinc.eu>
</commit_message>
<xml_diff>
--- a/Data Files/TestData/PermisosTestDataCasino.xlsx
+++ b/Data Files/TestData/PermisosTestDataCasino.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
   <si>
     <t xml:space="preserve">TestCaseId</t>
   </si>
@@ -101,6 +101,81 @@
   </si>
   <si>
     <t xml:space="preserve">Validación de permiso fallida por incumplimiento de verifaicación de elementos en la página </t>
+  </si>
+  <si>
+    <t>10/10/2019</t>
+  </si>
+  <si>
+    <t>13:43:35.246</t>
+  </si>
+  <si>
+    <t>Fallido</t>
+  </si>
+  <si>
+    <t>Validación de permiso fallida causado por excepción inesperada</t>
+  </si>
+  <si>
+    <t>13:43:53.134</t>
+  </si>
+  <si>
+    <t>13:51:21.654</t>
+  </si>
+  <si>
+    <t>Windows Server 2016</t>
+  </si>
+  <si>
+    <t>1920x1080</t>
+  </si>
+  <si>
+    <t>Firefox 69.0.2</t>
+  </si>
+  <si>
+    <t>Casino</t>
+  </si>
+  <si>
+    <t>Exitoso</t>
+  </si>
+  <si>
+    <t>Permiso Casino es correctamente accesible para el usuario</t>
+  </si>
+  <si>
+    <t>http://pregame-support.bminc.eu</t>
+  </si>
+  <si>
+    <t>4fku01</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>13:51:45.714</t>
+  </si>
+  <si>
+    <t>13:53:52.182</t>
+  </si>
+  <si>
+    <t>http://10.0.74.5/index/home</t>
+  </si>
+  <si>
+    <t>13:54:16.480</t>
+  </si>
+  <si>
+    <t>14:09:32.446</t>
+  </si>
+  <si>
+    <t>14:09:56.512</t>
+  </si>
+  <si>
+    <t>14:11:40.413</t>
+  </si>
+  <si>
+    <t>14:12:04.599</t>
+  </si>
+  <si>
+    <t>14:12:45.637</t>
+  </si>
+  <si>
+    <t>14:13:09.318</t>
   </si>
 </sst>
 </file>
@@ -287,22 +362,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="71.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="22.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="18.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="15"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="18.73" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="27.38" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="18.38" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="18.12" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="11.63" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="0" width="12.25" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="0" width="13.37" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="0" width="11.76" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="0" width="16.75" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="0" width="15.38" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="0" width="16.75" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="0" width="15.27" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="0" width="71.25" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="0" width="22.38" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="24" customWidth="true" hidden="false" style="0" width="18.73" collapsed="true" outlineLevel="0"/>
+    <col min="26" max="26" customWidth="true" hidden="false" style="0" width="15.0" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -354,44 +429,44 @@
       <c r="A2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>26</v>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>